<commit_message>
Update AUS and TWN scaling mappings. Remove AUS from UNFCCC scaling.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Australia_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Australia_scaling_mapping.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="13260" windowHeight="5775"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="17340" windowHeight="12980"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="215">
   <si>
     <t>iso</t>
   </si>
@@ -72,15 +77,6 @@
     <t>non-road transportation</t>
   </si>
   <si>
-    <t>waste-incineration</t>
-  </si>
-  <si>
-    <t>solid_waste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aviation </t>
-  </si>
-  <si>
     <t>metal_production</t>
   </si>
   <si>
@@ -99,9 +95,6 @@
     <t>power_plants</t>
   </si>
   <si>
-    <t>railway_etc</t>
-  </si>
-  <si>
     <t>Accommodation [*]</t>
   </si>
   <si>
@@ -504,9 +497,6 @@
     <t>Other-product-use</t>
   </si>
   <si>
-    <t>Other-process</t>
-  </si>
-  <si>
     <t>AGR</t>
   </si>
   <si>
@@ -624,9 +614,6 @@
     <t>2D_Paint-application</t>
   </si>
   <si>
-    <t>2L_Other-process-emissions</t>
-  </si>
-  <si>
     <t>1A3aii_Domestic-aviation</t>
   </si>
   <si>
@@ -637,13 +624,55 @@
   </si>
   <si>
     <t>1A3dii_Domestic-naviation</t>
+  </si>
+  <si>
+    <t>railway</t>
+  </si>
+  <si>
+    <t>Fugitive_Fossil_Fuels</t>
+  </si>
+  <si>
+    <t>1B1_Fugitive-solid-fuels</t>
+  </si>
+  <si>
+    <t>1B2_Fugitive-petr-and-gas</t>
+  </si>
+  <si>
+    <t>1B2d_Fugitive-other-energy</t>
+  </si>
+  <si>
+    <t>5D_Wastewater-handling</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Check Defn of this</t>
+  </si>
+  <si>
+    <t>2D3_Chemical-products-manufacture-processing</t>
+  </si>
+  <si>
+    <t>Not included in CEDS</t>
+  </si>
+  <si>
+    <t>1A5_Other-unspecified</t>
+  </si>
+  <si>
+    <t>Other-unspecified</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>Keep default since sector is not sufficently broken out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,6 +818,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1091,7 +1136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1151,8 +1196,124 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1214,12 +1375,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="175">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="47"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
@@ -1260,11 +1422,127 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1577,19 +1855,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
@@ -1599,239 +1880,242 @@
       <c r="C1" s="20" t="s">
         <v>13</v>
       </c>
+      <c r="E1" t="s">
+        <v>207</v>
+      </c>
       <c r="I1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="28" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="28" customFormat="1">
       <c r="A21" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="28" customFormat="1">
       <c r="A22" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="28" customFormat="1">
       <c r="A23" s="28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="28" customFormat="1">
       <c r="A24" s="28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="28" customFormat="1">
       <c r="A25" s="28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>15</v>
       </c>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="10" customFormat="1">
       <c r="A29" s="28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>15</v>
@@ -1839,282 +2123,292 @@
       <c r="F29"/>
       <c r="J29" s="28"/>
     </row>
-    <row r="30" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>146</v>
+    <row r="30" spans="1:10" s="28" customFormat="1">
+      <c r="A30" t="s">
+        <v>143</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F30"/>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" s="28" customFormat="1">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="F34" s="10"/>
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="J34" s="28"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:10" s="28" customFormat="1"/>
+    <row r="36" spans="1:10" ht="15">
+      <c r="A36" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="J36" s="28"/>
+    </row>
+    <row r="37" spans="1:10" ht="15">
+      <c r="A37" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="43"/>
+      <c r="F37" s="16"/>
+      <c r="J37" s="28"/>
+    </row>
+    <row r="38" spans="1:10" ht="15">
+      <c r="A38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:10" ht="15">
+      <c r="A39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A40" s="16"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="54" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="10" customFormat="1" ht="15">
+      <c r="A42" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A43" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A44" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A45" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A46" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A47" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A48" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15">
+      <c r="A49" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="28"/>
+    </row>
+    <row r="50" spans="1:10" ht="15">
+      <c r="A50" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="28"/>
+    </row>
+    <row r="51" spans="1:10" ht="15">
+      <c r="A51" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="28"/>
+    </row>
+    <row r="52" spans="1:10" ht="15">
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="28"/>
+    </row>
+    <row r="53" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A53" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15">
+      <c r="A54" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="28"/>
+    </row>
+    <row r="55" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15">
+      <c r="A56" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="28"/>
+    </row>
+    <row r="57" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A57" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A59" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="J62" s="28"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="16"/>
-      <c r="J35" s="28"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="16"/>
-    </row>
-    <row r="39" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40"/>
-      <c r="J40" s="28"/>
-    </row>
-    <row r="41" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42"/>
-    </row>
-    <row r="43" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="10"/>
-    </row>
-    <row r="46" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="28"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="28"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="28"/>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="28"/>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>123</v>
-      </c>
-      <c r="B51" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="28"/>
-    </row>
-    <row r="52" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="B53" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="J53" s="28"/>
-    </row>
-    <row r="54" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J61" s="28"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B62" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="C62" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B63" s="35" t="s">
-        <v>161</v>
+      <c r="B63" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="59" t="s">
+        <v>195</v>
       </c>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
@@ -2122,105 +2416,102 @@
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
-        <v>149</v>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="G64" s="21"/>
-    </row>
-    <row r="65" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>47</v>
+        <v>157</v>
+      </c>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="28" t="s">
+        <v>145</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="G65" s="21"/>
+    </row>
+    <row r="66" spans="1:10" s="28" customFormat="1">
+      <c r="A66" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="C66" s="28"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="1:10" s="28" customFormat="1">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="C67" s="28"/>
-    </row>
-    <row r="68" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>108</v>
-      </c>
-      <c r="B68" s="39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="63"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="28"/>
+    </row>
+    <row r="69" spans="1:10" s="28" customFormat="1">
+      <c r="B69" s="62"/>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C70" s="60" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="63"/>
-      <c r="C71" s="63"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B72" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C72" s="58" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D73"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" s="44" t="s">
-        <v>169</v>
-      </c>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="28"/>
+    </row>
+    <row r="72" spans="1:10" s="28" customFormat="1">
+      <c r="B72" s="62"/>
+      <c r="C72" s="62"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="28" customFormat="1">
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
@@ -2228,14 +2519,16 @@
       <c r="H74"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B75" s="25" t="s">
+    <row r="75" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A75" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C75"/>
+      <c r="C75" s="44" t="s">
+        <v>164</v>
+      </c>
       <c r="D75"/>
       <c r="E75"/>
       <c r="F75"/>
@@ -2243,225 +2536,240 @@
       <c r="H75"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" s="28" t="s">
+    <row r="76" spans="1:10" s="28" customFormat="1">
+      <c r="A76" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J76" s="28"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="J77" s="28"/>
     </row>
-    <row r="78" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="24" t="s">
+    <row r="78" spans="1:10">
+      <c r="J78" s="28"/>
+    </row>
+    <row r="79" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A79" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="28" customFormat="1">
+      <c r="A80" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="28"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+    </row>
+    <row r="82" spans="1:10" s="28" customFormat="1">
+      <c r="A82" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" s="26"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:10" ht="15">
+      <c r="A83" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C78" s="29" t="s">
+      <c r="B83" s="28"/>
+      <c r="C83" s="63" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="28" customFormat="1">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84"/>
+    </row>
+    <row r="85" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A85" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A86" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+    </row>
+    <row r="87" spans="1:10" ht="15">
+      <c r="A87" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="28"/>
+    </row>
+    <row r="88" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A88" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+    </row>
+    <row r="89" spans="1:10" ht="15">
+      <c r="A89" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B89" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+    </row>
+    <row r="90" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A90" t="s">
+        <v>57</v>
+      </c>
+      <c r="B90" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A91" t="s">
+        <v>110</v>
+      </c>
+      <c r="B91" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="15">
+      <c r="A92" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J92" s="28"/>
+    </row>
+    <row r="93" spans="1:10" s="28" customFormat="1"/>
+    <row r="94" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A94" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A95" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="45" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C79"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
-      <c r="B80" s="28"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
-    </row>
-    <row r="81" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B81" s="26" t="s">
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+    </row>
+    <row r="96" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A96" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B82" s="28" t="s">
+      <c r="C96" s="64" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+    </row>
+    <row r="97" spans="1:10" s="28" customFormat="1">
+      <c r="A97" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" s="28" t="s">
         <v>20</v>
-      </c>
-      <c r="C82" s="64" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="52" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>135</v>
-      </c>
-      <c r="B86" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-    </row>
-    <row r="87" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="B87" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D87"/>
-      <c r="E87"/>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B88" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="28"/>
-      <c r="H88" s="28"/>
-      <c r="I88" s="28"/>
-    </row>
-    <row r="89" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>61</v>
-      </c>
-      <c r="B89" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>114</v>
-      </c>
-      <c r="B90" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B92" t="s">
-        <v>18</v>
-      </c>
-      <c r="C92" s="57" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="B93" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" s="56" t="s">
-        <v>197</v>
-      </c>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B94" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" s="28"/>
-      <c r="J94" s="28"/>
-    </row>
-    <row r="95" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B96" t="s">
-        <v>23</v>
-      </c>
-      <c r="C96" s="53" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B97" s="28" t="s">
-        <v>23</v>
       </c>
       <c r="D97"/>
       <c r="E97"/>
@@ -2470,41 +2778,43 @@
       <c r="H97"/>
       <c r="I97"/>
     </row>
-    <row r="98" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="28" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C98"/>
-      <c r="D98"/>
-      <c r="E98"/>
-      <c r="F98"/>
-      <c r="G98"/>
-      <c r="H98"/>
-      <c r="I98"/>
-    </row>
-    <row r="99" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
-        <v>87</v>
+        <v>20</v>
+      </c>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" t="s">
+        <v>60</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D99"/>
-      <c r="E99"/>
-      <c r="F99"/>
-      <c r="G99"/>
-      <c r="H99"/>
-      <c r="I99"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="28" t="s">
-        <v>127</v>
+        <v>20</v>
+      </c>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" t="s">
+        <v>109</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -2513,560 +2823,531 @@
       <c r="G100" s="28"/>
       <c r="H100" s="28"/>
       <c r="I100" s="28"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J100" s="28"/>
+    </row>
+    <row r="101" spans="1:10" s="28" customFormat="1">
       <c r="A101" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="28" customFormat="1"/>
+    <row r="103" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A103" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C103" s="49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="A104" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C104" s="50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15">
+      <c r="A105" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C105" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="J105" s="28"/>
+    </row>
+    <row r="106" spans="1:10" ht="15">
+      <c r="A106" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B106" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="J106" s="28"/>
+    </row>
+    <row r="107" spans="1:10" ht="15">
+      <c r="A107" t="s">
         <v>64</v>
       </c>
-      <c r="B101" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B107" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C107" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="J107" s="28"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="28"/>
+      <c r="I108" s="28"/>
+      <c r="J108" s="28"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="28"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="28"/>
+      <c r="I109" s="28"/>
+      <c r="J109" s="28"/>
+    </row>
+    <row r="110" spans="1:10" ht="15">
+      <c r="A110" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C110" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="J110" s="28"/>
+    </row>
+    <row r="111" spans="1:10" ht="15">
+      <c r="A111" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B111" s="28"/>
+      <c r="C111" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="J111" s="28"/>
+    </row>
+    <row r="112" spans="1:10" ht="15">
+      <c r="A112" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B112" s="28"/>
+      <c r="C112" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="J112" s="28"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
+      <c r="J113" s="28"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B102" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="28"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
-    </row>
-    <row r="103" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B114" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J114" s="28"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J115" s="28"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J116" s="28"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="15">
+      <c r="A118" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" s="45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="15">
+      <c r="A119" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B103" s="28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>66</v>
-      </c>
-      <c r="B104" s="28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="B106" t="s">
-        <v>24</v>
-      </c>
-      <c r="C106" s="49" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>118</v>
-      </c>
-      <c r="B107" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C107" s="50" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B108" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C108" s="51" t="s">
-        <v>189</v>
-      </c>
-      <c r="J108" s="28"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B109" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J109" s="28"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>68</v>
-      </c>
-      <c r="B110" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J110" s="28"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>78</v>
-      </c>
-      <c r="B111" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" s="28"/>
-      <c r="E111" s="28"/>
-      <c r="F111" s="28"/>
-      <c r="G111" s="28"/>
-      <c r="H111" s="28"/>
-      <c r="I111" s="28"/>
-      <c r="J111" s="28"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="28"/>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-      <c r="F112" s="28"/>
-      <c r="G112" s="28"/>
-      <c r="H112" s="28"/>
-      <c r="I112" s="28"/>
-      <c r="J112" s="28"/>
-    </row>
-    <row r="113" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C113" s="62" t="s">
-        <v>203</v>
-      </c>
-      <c r="J113" s="28"/>
-    </row>
-    <row r="114" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B114" s="28"/>
-      <c r="C114" s="62" t="s">
-        <v>204</v>
-      </c>
-      <c r="J114" s="28"/>
-    </row>
-    <row r="115" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="B115" s="28"/>
-      <c r="C115" s="62" t="s">
-        <v>205</v>
-      </c>
-      <c r="J115" s="28"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="28"/>
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="J116" s="28"/>
-    </row>
-    <row r="117" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B117" t="s">
-        <v>25</v>
-      </c>
-      <c r="C117" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="J117" s="28"/>
-    </row>
-    <row r="118" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B118" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C118" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="J118" s="28"/>
-    </row>
-    <row r="119" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="28" t="s">
-        <v>106</v>
-      </c>
       <c r="B119" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C119" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="J119" s="28"/>
-    </row>
-    <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:10" ht="15">
       <c r="A120" s="28" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C120" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="J120" s="28"/>
-    </row>
-    <row r="121" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="28" t="s">
-        <v>104</v>
+    </row>
+    <row r="121" spans="1:10" ht="15">
+      <c r="A121" t="s">
+        <v>75</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C121" s="45" t="s">
         <v>174</v>
       </c>
       <c r="J121" s="28"/>
     </row>
-    <row r="122" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="28" t="s">
-        <v>96</v>
+    <row r="122" spans="1:10">
+      <c r="A122" t="s">
+        <v>67</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C122" s="45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="28" t="s">
-        <v>151</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" t="s">
+        <v>68</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C123" s="45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="28" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C124" s="45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="15">
       <c r="A125" s="28" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C125" s="45" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J125" s="28"/>
+    </row>
+    <row r="126" spans="1:10" ht="15">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C126" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" s="46"/>
+      <c r="J126" s="28"/>
+    </row>
+    <row r="127" spans="1:10" ht="15">
+      <c r="A127" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B127" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C127" s="45"/>
+      <c r="J127" s="28"/>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" t="s">
+        <v>85</v>
+      </c>
+      <c r="B128" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J128" s="28"/>
+    </row>
+    <row r="129" spans="1:10" ht="15">
+      <c r="C129" s="45"/>
+      <c r="J129" s="28"/>
+    </row>
+    <row r="130" spans="1:10" ht="15">
+      <c r="A130" t="s">
+        <v>81</v>
+      </c>
+      <c r="B130" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C130" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J130" s="28"/>
+    </row>
+    <row r="131" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="B131" s="48"/>
+      <c r="C131" s="48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="J132" s="28"/>
+    </row>
+    <row r="133" spans="1:10" ht="15">
+      <c r="A133" t="s">
+        <v>120</v>
+      </c>
+      <c r="B133" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C133" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="J126" s="28"/>
-    </row>
-    <row r="127" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="J133" s="28"/>
+    </row>
+    <row r="134" spans="1:10" ht="15">
+      <c r="A134" t="s">
+        <v>121</v>
+      </c>
+      <c r="B134" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="J134" s="28"/>
+    </row>
+    <row r="135" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="B135" s="63"/>
+    </row>
+    <row r="136" spans="1:10" ht="15">
+      <c r="A136" t="s">
+        <v>108</v>
+      </c>
+      <c r="B136" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="C136" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="J136" s="28"/>
+    </row>
+    <row r="137" spans="1:10" ht="15">
+      <c r="A137" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B127" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C127" s="45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>72</v>
-      </c>
-      <c r="B128" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C128" s="45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B129" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C129" s="45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B130" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C130" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="J130" s="28"/>
-    </row>
-    <row r="131" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>111</v>
-      </c>
-      <c r="B131" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C131" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="J131" s="28"/>
-    </row>
-    <row r="132" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B132" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C132" s="45"/>
-      <c r="J132" s="28"/>
-    </row>
-    <row r="133" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C133" s="45"/>
-      <c r="J133" s="28"/>
-    </row>
-    <row r="134" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>85</v>
-      </c>
-      <c r="B134" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C134" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="J134" s="28"/>
-    </row>
-    <row r="135" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B135" s="48"/>
-      <c r="C135" s="48" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J136" s="28"/>
-    </row>
-    <row r="137" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>124</v>
-      </c>
-      <c r="B137" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C137" s="47" t="s">
-        <v>184</v>
+      <c r="B137" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="C137" s="64" t="s">
+        <v>204</v>
       </c>
       <c r="J137" s="28"/>
     </row>
-    <row r="138" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="138" spans="1:10" ht="15">
+      <c r="B138" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="C138" s="64" t="s">
+        <v>205</v>
+      </c>
+      <c r="J138" s="28"/>
+    </row>
+    <row r="139" spans="1:10" ht="15">
+      <c r="A139" t="s">
+        <v>149</v>
+      </c>
+      <c r="B139" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="J139" s="28"/>
+    </row>
+    <row r="140" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="C140" s="64"/>
+    </row>
+    <row r="141" spans="1:10" ht="15">
+      <c r="A141" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B138" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J138" s="28"/>
-    </row>
-    <row r="139" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>112</v>
-      </c>
-      <c r="B139" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J139" s="28"/>
-    </row>
-    <row r="140" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>89</v>
-      </c>
-      <c r="B140" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J140" s="28"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>158</v>
+      </c>
+      <c r="C141" s="55" t="s">
+        <v>188</v>
+      </c>
       <c r="J141" s="28"/>
     </row>
-    <row r="142" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="15">
       <c r="A142" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B142" t="s">
-        <v>163</v>
+      <c r="B142" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="C142" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J142" s="28"/>
+    </row>
+    <row r="143" spans="1:10" ht="15">
+      <c r="A143" t="s">
+        <v>112</v>
+      </c>
+      <c r="B143" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C143" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="J143" s="28"/>
+    </row>
+    <row r="144" spans="1:10" ht="15">
+      <c r="B144" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C144" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="J144" s="28"/>
+    </row>
+    <row r="145" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="C145" s="55"/>
+    </row>
+    <row r="146" spans="1:10" ht="15">
+      <c r="A146" t="s">
+        <v>78</v>
+      </c>
+      <c r="B146" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="C146" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="J146" s="28"/>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B147" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="J147" s="28"/>
+    </row>
+    <row r="148" spans="1:10">
+      <c r="B148" s="40"/>
+      <c r="J148" s="28"/>
+    </row>
+    <row r="149" spans="1:10" s="16" customFormat="1" ht="15">
+      <c r="A149" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B149" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="C149" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="E149" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="F149"/>
+      <c r="J149" s="28"/>
+    </row>
+    <row r="150" spans="1:10" ht="15">
+      <c r="A150" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B150" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="C150" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="J150" s="28"/>
+    </row>
+    <row r="151" spans="1:10" ht="15">
+      <c r="A151" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B151" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="C151" s="28"/>
+    </row>
+    <row r="152" spans="1:10" ht="15">
+      <c r="A152" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C152" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="J142" s="28"/>
-    </row>
-    <row r="143" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B143" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="C143" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="J143" s="28"/>
-    </row>
-    <row r="144" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>116</v>
-      </c>
-      <c r="B144" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="C144" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="J144" s="28"/>
-    </row>
-    <row r="145" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B145" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="C145" s="55" t="s">
-        <v>196</v>
-      </c>
-      <c r="J145" s="28"/>
-    </row>
-    <row r="146" spans="1:10" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C146" s="55"/>
-    </row>
-    <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>82</v>
-      </c>
-      <c r="B147" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="C147" s="61" t="s">
-        <v>202</v>
-      </c>
-      <c r="J147" s="28"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B148" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J148" s="28"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B149" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J149" s="28"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>153</v>
-      </c>
-      <c r="B150" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J150" s="28"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>101</v>
-      </c>
-      <c r="B151" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J151" s="28"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B152" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J152" s="28"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>93</v>
-      </c>
-      <c r="B153" s="40" t="s">
-        <v>162</v>
-      </c>
+      <c r="E152" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="J153" s="28"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
+      <c r="A154" t="s">
+        <v>62</v>
+      </c>
+      <c r="E154" t="s">
+        <v>210</v>
+      </c>
       <c r="J154" s="28"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
+      <c r="A155" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E155" s="28" t="s">
+        <v>210</v>
+      </c>
       <c r="J155" s="28"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="J156" s="28"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J157" s="28"/>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J158" s="28"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J159" s="28"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J160" s="28"/>
     </row>
   </sheetData>
   <sortState ref="J1:J155">
     <sortCondition ref="J1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3078,9 +3359,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3100,7 +3381,7 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -3122,6 +3403,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3133,9 +3419,9 @@
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3161,7 +3447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
@@ -3187,5 +3473,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>